<commit_message>
added option to filter out blanks growing absorption
</commit_message>
<xml_diff>
--- a/data-raw/mapa_test.xlsx
+++ b/data-raw/mapa_test.xlsx
@@ -124,12 +124,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -142,10 +142,10 @@
   <dimension ref="A1:U24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+      <selection pane="topLeft" activeCell="U13" activeCellId="0" sqref="U13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.44"/>
@@ -159,10 +159,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="5.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="15.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="5.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="5.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="15" style="0" width="4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="22" style="0" width="8.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>